<commit_message>
i486--suite file macro non-matched support
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite2/radiant_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite2/radiant_regression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_example\standard_suite2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF3C50A-5323-499C-A0AF-FAA03A953395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF7EE93-7FB7-434C-8765-7F8D2C277C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite_eng" sheetId="1" r:id="rId1"/>
@@ -32,15 +32,15 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="370">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1179,6 +1179,9 @@
   </si>
   <si>
     <t>estimated memory usage for task case run, dynamic based on current system available memoroy</t>
+  </si>
+  <si>
+    <t>Macro section negative match support</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1687,37 +1690,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1784,52 +1756,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="34" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
@@ -1839,7 +1774,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
@@ -1970,21 +1905,6 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2000,10 +1920,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="32" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2031,9 +1951,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -2088,139 +2005,115 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="5" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="32" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2781,6 +2674,23 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -2863,7 +2773,19 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> modelsim</a:t>
+            <a:t> modelsim    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>or     !=questasim</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -3151,7 +3073,61 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>		Expression:currently we only support expression start with "=",  the sorting value can be one or more (Separated with ",").  The value in case sheet must be same or one of the condition given values. </a:t>
+            <a:t>		Expression:currently we support expression start with "="and "!=",  the sorting value can be one or more (Separated with ",").  </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			"=": The value in case sheet should match one of condition given values.   </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			"!=": The value in case sheet should not match any of condition given values.    </a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -4885,9 +4861,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4925,9 +4901,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4960,26 +4936,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5012,26 +4971,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5209,184 +5151,184 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" style="52" customWidth="1"/>
-    <col min="2" max="2" width="28" style="52" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="52"/>
+    <col min="1" max="1" width="15" style="47" customWidth="1"/>
+    <col min="2" max="2" width="28" style="47" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="47" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="47" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="47" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="47" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="47" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="47" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="47" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="47" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="47" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="47" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="47" t="s">
         <v>336</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="47" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="47" t="s">
         <v>336</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="47" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="47" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="47" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="47" t="s">
         <v>336</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="47" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="47" t="s">
         <v>336</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="47" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="47" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="47" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="47" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B41" sqref="B41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5395,8 +5337,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B41" sqref="B41"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5416,111 +5358,111 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" style="52" customWidth="1"/>
-    <col min="2" max="2" width="28" style="52" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="52"/>
+    <col min="1" max="1" width="15" style="47" customWidth="1"/>
+    <col min="2" max="2" width="28" style="47" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="47" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="47" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="47" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="47" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="47" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="47" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="47" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="47" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="47" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="47" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="47" t="s">
         <v>336</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="47" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="47" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="47" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5545,344 +5487,344 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="9" style="52" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="52" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="52" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="52" customWidth="1"/>
-    <col min="7" max="7" width="24" style="52" customWidth="1"/>
-    <col min="8" max="8" width="37" style="52" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="52" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="52" customWidth="1"/>
-    <col min="11" max="11" width="12" style="52" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="53" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="53" customWidth="1"/>
-    <col min="14" max="14" width="38" style="52" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="52" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="52" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="52" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="52" customWidth="1"/>
-    <col min="19" max="19" width="13" style="52" customWidth="1"/>
-    <col min="20" max="21" width="9.7109375" style="52" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="52" customWidth="1"/>
-    <col min="23" max="23" width="11" style="52" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" style="52" customWidth="1"/>
-    <col min="25" max="30" width="9" style="52"/>
-    <col min="31" max="31" width="10.140625" style="52" customWidth="1"/>
-    <col min="32" max="16384" width="9" style="52"/>
+    <col min="1" max="1" width="10.28515625" style="47" customWidth="1"/>
+    <col min="2" max="2" width="9" style="47" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" style="47" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="47" customWidth="1"/>
+    <col min="7" max="7" width="24" style="47" customWidth="1"/>
+    <col min="8" max="8" width="37" style="47" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="47" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="47" customWidth="1"/>
+    <col min="11" max="11" width="12" style="47" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="48" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="48" customWidth="1"/>
+    <col min="14" max="14" width="38" style="47" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="47" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="47" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="47" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="47" customWidth="1"/>
+    <col min="19" max="19" width="13" style="47" customWidth="1"/>
+    <col min="20" max="21" width="9.7109375" style="47" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="47" customWidth="1"/>
+    <col min="23" max="23" width="11" style="47" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" style="47" customWidth="1"/>
+    <col min="25" max="30" width="9" style="47"/>
+    <col min="31" max="31" width="10.140625" style="47" customWidth="1"/>
+    <col min="32" max="16384" width="9" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="51" customFormat="1">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:32" s="46" customFormat="1">
+      <c r="A1" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="92"/>
-      <c r="Y1" s="93" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93"/>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93"/>
-      <c r="AF1" s="93"/>
-    </row>
-    <row r="2" spans="1:32" s="51" customFormat="1">
-      <c r="A2" s="54" t="s">
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
+    </row>
+    <row r="2" spans="1:32" s="46" customFormat="1">
+      <c r="A2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="M2" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="N2" s="54" t="s">
+      <c r="N2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="O2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="54" t="s">
+      <c r="P2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="54" t="s">
+      <c r="Q2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="54" t="s">
+      <c r="R2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="54" t="s">
+      <c r="S2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="54" t="s">
+      <c r="T2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="V2" s="54" t="s">
+      <c r="V2" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="54" t="s">
+      <c r="W2" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="54" t="s">
+      <c r="X2" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="54" t="s">
+      <c r="Z2" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="54" t="s">
+      <c r="AA2" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" s="54" t="s">
+      <c r="AB2" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="54" t="s">
+      <c r="AC2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="54" t="s">
+      <c r="AD2" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="54" t="s">
+      <c r="AE2" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="54" t="s">
+      <c r="AF2" s="49" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:32">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="52" t="s">
+      <c r="P3" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="AF3" s="52" t="s">
+      <c r="AF3" s="47" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>330</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="52" t="s">
+      <c r="T4" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="AF4" s="52" t="s">
+      <c r="AF4" s="47" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="47" t="s">
         <v>331</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="52" t="s">
+      <c r="T5" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="AF5" s="52" t="s">
+      <c r="AF5" s="47" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="47" t="s">
         <v>332</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="T6" s="52" t="s">
+      <c r="T6" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="AF6" s="52" t="s">
+      <c r="AF6" s="47" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="47" t="s">
         <v>333</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="47" t="s">
         <v>353</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="47" t="s">
         <v>353</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="47" t="s">
         <v>329</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="T7" s="52" t="s">
+      <c r="T7" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="AF7" s="52" t="s">
+      <c r="AF7" s="47" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:32">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="47" t="s">
         <v>329</v>
       </c>
-      <c r="H8" s="52" t="s">
+      <c r="H8" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="T8" s="52" t="s">
+      <c r="T8" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="AF8" s="52" t="s">
+      <c r="AF8" s="47" t="s">
         <v>341</v>
       </c>
     </row>
@@ -5890,26 +5832,26 @@
   <sheetProtection algorithmName="SHA-512" hashValue="Sju3pjEnjegba3BrZLImZ+xscQ9MLEq+i8mDO7rXFn4S3yXv8zWb4HaF0uC2YruSs8wkV8FCIxY7a0fvnwVXFw==" saltValue="mZmUchosJ60PlKqUXOSzGQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AF45" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{BDC83C48-43E8-4F85-A58B-3C1DF7812A62}"/>
+      <autoFilter ref="A2:AF46" xr:uid="{C9888BD5-80EC-4D9A-BEF0-EBC8ED55A72B}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
       <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{692EE2CB-742F-4DA8-AAFC-9AF6C50F791E}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{1D9B52B8-7B9F-4231-9249-EB767C5CD2A6}"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AF46" xr:uid="{6228A706-72E8-415D-BB22-48C6325FF00D}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{3F971DA5-1E37-4E46-8EBD-E3C79E3D44B6}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -6002,193 +5944,193 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="9" style="52" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="52" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="52" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="52" customWidth="1"/>
-    <col min="7" max="7" width="24" style="52" customWidth="1"/>
-    <col min="8" max="8" width="37" style="52" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="52" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="52" customWidth="1"/>
-    <col min="11" max="11" width="12" style="52" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="53" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="53" customWidth="1"/>
-    <col min="14" max="14" width="38" style="52" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="52" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="52" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="52" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="52" customWidth="1"/>
-    <col min="19" max="19" width="13" style="52" customWidth="1"/>
-    <col min="20" max="21" width="9.7109375" style="52" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="52" customWidth="1"/>
-    <col min="23" max="23" width="11" style="52" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" style="52" customWidth="1"/>
-    <col min="25" max="30" width="9" style="52"/>
-    <col min="31" max="31" width="10.140625" style="52" customWidth="1"/>
-    <col min="32" max="16384" width="9" style="52"/>
+    <col min="1" max="1" width="10.28515625" style="47" customWidth="1"/>
+    <col min="2" max="2" width="9" style="47" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" style="47" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="47" customWidth="1"/>
+    <col min="7" max="7" width="24" style="47" customWidth="1"/>
+    <col min="8" max="8" width="37" style="47" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="47" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="47" customWidth="1"/>
+    <col min="11" max="11" width="12" style="47" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="48" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="48" customWidth="1"/>
+    <col min="14" max="14" width="38" style="47" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="47" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="47" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="47" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="47" customWidth="1"/>
+    <col min="19" max="19" width="13" style="47" customWidth="1"/>
+    <col min="20" max="21" width="9.7109375" style="47" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="47" customWidth="1"/>
+    <col min="23" max="23" width="11" style="47" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" style="47" customWidth="1"/>
+    <col min="25" max="30" width="9" style="47"/>
+    <col min="31" max="31" width="10.140625" style="47" customWidth="1"/>
+    <col min="32" max="16384" width="9" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="51" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:32" s="46" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A1" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="92"/>
-      <c r="Y1" s="93" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93"/>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93"/>
-      <c r="AF1" s="93"/>
-    </row>
-    <row r="2" spans="1:32" s="51" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A2" s="54" t="s">
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
+    </row>
+    <row r="2" spans="1:32" s="46" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="M2" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="N2" s="54" t="s">
+      <c r="N2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="O2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="54" t="s">
+      <c r="P2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="54" t="s">
+      <c r="Q2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="54" t="s">
+      <c r="R2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="54" t="s">
+      <c r="S2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="54" t="s">
+      <c r="T2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="V2" s="54" t="s">
+      <c r="V2" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="54" t="s">
+      <c r="W2" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="54" t="s">
+      <c r="X2" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="54" t="s">
+      <c r="Z2" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="54" t="s">
+      <c r="AA2" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" s="54" t="s">
+      <c r="AB2" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="54" t="s">
+      <c r="AC2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="54" t="s">
+      <c r="AD2" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="54" t="s">
+      <c r="AE2" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="54" t="s">
+      <c r="AF2" s="49" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15.75" thickTop="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="47" t="s">
         <v>339</v>
       </c>
     </row>
@@ -6275,10 +6217,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N283"/>
+  <dimension ref="A1:N284"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F161" sqref="F161"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6301,7 +6243,7 @@
         <v>53</v>
       </c>
       <c r="B1" s="2">
-        <v>1.28</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6309,7 +6251,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="3">
-        <v>45063</v>
+        <v>45306</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
@@ -6339,17 +6281,17 @@
       <c r="E111" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F111" s="125" t="s">
+      <c r="F111" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="G111" s="126"/>
-      <c r="H111" s="126"/>
-      <c r="I111" s="126"/>
-      <c r="J111" s="126"/>
-      <c r="K111" s="126"/>
-      <c r="L111" s="126"/>
-      <c r="M111" s="126"/>
-      <c r="N111" s="127"/>
+      <c r="G111" s="83"/>
+      <c r="H111" s="83"/>
+      <c r="I111" s="83"/>
+      <c r="J111" s="83"/>
+      <c r="K111" s="83"/>
+      <c r="L111" s="83"/>
+      <c r="M111" s="83"/>
+      <c r="N111" s="84"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -6926,7 +6868,7 @@
       <c r="N132" s="11"/>
     </row>
     <row r="133" spans="1:14">
-      <c r="A133" s="61" t="s">
+      <c r="A133" s="56" t="s">
         <v>237</v>
       </c>
       <c r="B133" s="9" t="s">
@@ -6938,7 +6880,7 @@
       <c r="D133" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E133" s="62" t="s">
+      <c r="E133" s="57" t="s">
         <v>238</v>
       </c>
       <c r="F133" s="9"/>
@@ -7240,51 +7182,51 @@
       </c>
     </row>
     <row r="148" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A148" s="80" t="s">
+      <c r="A148" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="B148" s="81" t="s">
+      <c r="B148" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C148" s="81" t="s">
+      <c r="C148" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="D148" s="81" t="s">
+      <c r="D148" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="E148" s="81" t="s">
+      <c r="E148" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="F148" s="81" t="s">
+      <c r="F148" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="G148" s="81" t="s">
+      <c r="G148" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="H148" s="82" t="s">
+      <c r="H148" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="149" spans="1:8">
-      <c r="A149" s="75">
+      <c r="A149" s="69">
         <v>1</v>
       </c>
-      <c r="B149" s="95" t="s">
+      <c r="B149" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C149" s="76" t="s">
+      <c r="C149" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="D149" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="E149" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="F149" s="74" t="s">
+      <c r="D149" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="E149" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="F149" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="G149" s="74" t="s">
+      <c r="G149" s="68" t="s">
         <v>91</v>
       </c>
       <c r="H149" s="1" t="s">
@@ -7295,7 +7237,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="96"/>
+      <c r="B150" s="110"/>
       <c r="C150" s="21" t="s">
         <v>93</v>
       </c>
@@ -7317,7 +7259,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="96"/>
+      <c r="B151" s="110"/>
       <c r="C151" s="21" t="s">
         <v>16</v>
       </c>
@@ -7337,7 +7279,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="96"/>
+      <c r="B152" s="110"/>
       <c r="C152" s="21" t="s">
         <v>95</v>
       </c>
@@ -7361,8 +7303,8 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="96"/>
-      <c r="C153" s="56" t="s">
+      <c r="B153" s="110"/>
+      <c r="C153" s="51" t="s">
         <v>97</v>
       </c>
       <c r="D153" s="21" t="s">
@@ -7385,8 +7327,8 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="96"/>
-      <c r="C154" s="56" t="s">
+      <c r="B154" s="110"/>
+      <c r="C154" s="51" t="s">
         <v>101</v>
       </c>
       <c r="D154" s="21" t="s">
@@ -7398,7 +7340,7 @@
       <c r="F154" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="G154" s="56" t="s">
+      <c r="G154" s="51" t="s">
         <v>224</v>
       </c>
       <c r="H154" s="11" t="s">
@@ -7409,7 +7351,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="96"/>
+      <c r="B155" s="110"/>
       <c r="C155" s="21" t="s">
         <v>103</v>
       </c>
@@ -7431,8 +7373,8 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="96"/>
-      <c r="C156" s="56" t="s">
+      <c r="B156" s="110"/>
+      <c r="C156" s="51" t="s">
         <v>104</v>
       </c>
       <c r="D156" s="21" t="s">
@@ -7455,8 +7397,8 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="96"/>
-      <c r="C157" s="56" t="s">
+      <c r="B157" s="110"/>
+      <c r="C157" s="51" t="s">
         <v>105</v>
       </c>
       <c r="D157" s="21" t="s">
@@ -7479,7 +7421,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="96"/>
+      <c r="B158" s="110"/>
       <c r="C158" s="21" t="s">
         <v>106</v>
       </c>
@@ -7492,7 +7434,7 @@
       <c r="F158" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="G158" s="56" t="s">
+      <c r="G158" s="51" t="s">
         <v>224</v>
       </c>
       <c r="H158" s="11" t="s">
@@ -7503,7 +7445,7 @@
       <c r="A159" s="19">
         <v>11</v>
       </c>
-      <c r="B159" s="96"/>
+      <c r="B159" s="110"/>
       <c r="C159" s="21" t="s">
         <v>107</v>
       </c>
@@ -7527,7 +7469,7 @@
       <c r="A160" s="19">
         <v>12</v>
       </c>
-      <c r="B160" s="96"/>
+      <c r="B160" s="110"/>
       <c r="C160" s="21" t="s">
         <v>109</v>
       </c>
@@ -7549,21 +7491,21 @@
       <c r="A161" s="19">
         <v>13</v>
       </c>
-      <c r="B161" s="96"/>
-      <c r="C161" s="56" t="s">
+      <c r="B161" s="110"/>
+      <c r="C161" s="51" t="s">
         <v>312</v>
       </c>
       <c r="D161" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E161" s="21"/>
-      <c r="F161" s="56" t="s">
+      <c r="F161" s="51" t="s">
         <v>367</v>
       </c>
-      <c r="G161" s="56" t="s">
+      <c r="G161" s="51" t="s">
         <v>366</v>
       </c>
-      <c r="H161" s="59" t="s">
+      <c r="H161" s="54" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7571,21 +7513,21 @@
       <c r="A162" s="19">
         <v>14</v>
       </c>
-      <c r="B162" s="96"/>
-      <c r="C162" s="56" t="s">
+      <c r="B162" s="110"/>
+      <c r="C162" s="51" t="s">
         <v>361</v>
       </c>
       <c r="D162" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E162" s="21"/>
-      <c r="F162" s="56" t="s">
+      <c r="F162" s="51" t="s">
         <v>365</v>
       </c>
-      <c r="G162" s="56" t="s">
+      <c r="G162" s="51" t="s">
         <v>362</v>
       </c>
-      <c r="H162" s="59" t="s">
+      <c r="H162" s="54" t="s">
         <v>363</v>
       </c>
     </row>
@@ -7593,7 +7535,7 @@
       <c r="A163" s="19">
         <v>15</v>
       </c>
-      <c r="B163" s="102"/>
+      <c r="B163" s="105"/>
       <c r="C163" s="21" t="s">
         <v>113</v>
       </c>
@@ -7617,7 +7559,7 @@
       <c r="A164" s="19">
         <v>16</v>
       </c>
-      <c r="B164" s="105" t="s">
+      <c r="B164" s="94" t="s">
         <v>4</v>
       </c>
       <c r="C164" s="21" t="s">
@@ -7635,17 +7577,17 @@
       <c r="G164" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="H164" s="59" t="s">
+      <c r="H164" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="I164" s="64"/>
+      <c r="I164" s="59"/>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="19">
         <v>17</v>
       </c>
-      <c r="B165" s="105"/>
-      <c r="C165" s="56" t="s">
+      <c r="B165" s="94"/>
+      <c r="C165" s="51" t="s">
         <v>256</v>
       </c>
       <c r="D165" s="21" t="s">
@@ -7654,13 +7596,13 @@
       <c r="E165" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F165" s="60" t="s">
+      <c r="F165" s="55" t="s">
         <v>257</v>
       </c>
-      <c r="G165" s="56" t="s">
+      <c r="G165" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H165" s="59" t="s">
+      <c r="H165" s="54" t="s">
         <v>261</v>
       </c>
     </row>
@@ -7668,8 +7610,8 @@
       <c r="A166" s="19">
         <v>18</v>
       </c>
-      <c r="B166" s="105"/>
-      <c r="C166" s="56" t="s">
+      <c r="B166" s="94"/>
+      <c r="C166" s="51" t="s">
         <v>259</v>
       </c>
       <c r="D166" s="21" t="s">
@@ -7678,13 +7620,13 @@
       <c r="E166" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F166" s="60" t="s">
+      <c r="F166" s="55" t="s">
         <v>258</v>
       </c>
-      <c r="G166" s="56" t="s">
+      <c r="G166" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H166" s="59" t="s">
+      <c r="H166" s="54" t="s">
         <v>260</v>
       </c>
     </row>
@@ -7692,8 +7634,8 @@
       <c r="A167" s="19">
         <v>19</v>
       </c>
-      <c r="B167" s="105"/>
-      <c r="C167" s="68" t="s">
+      <c r="B167" s="94"/>
+      <c r="C167" s="62" t="s">
         <v>292</v>
       </c>
       <c r="D167" s="21" t="s">
@@ -7702,13 +7644,13 @@
       <c r="E167" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F167" s="60">
+      <c r="F167" s="55">
         <v>0</v>
       </c>
-      <c r="G167" s="68" t="s">
+      <c r="G167" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="H167" s="69" t="s">
+      <c r="H167" s="63" t="s">
         <v>296</v>
       </c>
     </row>
@@ -7716,8 +7658,8 @@
       <c r="A168" s="19">
         <v>20</v>
       </c>
-      <c r="B168" s="105"/>
-      <c r="C168" s="68" t="s">
+      <c r="B168" s="94"/>
+      <c r="C168" s="62" t="s">
         <v>293</v>
       </c>
       <c r="D168" s="21" t="s">
@@ -7726,20 +7668,20 @@
       <c r="E168" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F168" s="60">
+      <c r="F168" s="55">
         <v>0</v>
       </c>
-      <c r="G168" s="68" t="s">
+      <c r="G168" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="H168" s="69"/>
+      <c r="H168" s="63"/>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="19">
         <v>21</v>
       </c>
-      <c r="B169" s="105"/>
-      <c r="C169" s="68" t="s">
+      <c r="B169" s="94"/>
+      <c r="C169" s="62" t="s">
         <v>294</v>
       </c>
       <c r="D169" s="21" t="s">
@@ -7748,20 +7690,20 @@
       <c r="E169" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F169" s="60">
+      <c r="F169" s="55">
         <v>1</v>
       </c>
-      <c r="G169" s="68" t="s">
+      <c r="G169" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="H169" s="59"/>
+      <c r="H169" s="54"/>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="19">
         <v>22</v>
       </c>
-      <c r="B170" s="105"/>
-      <c r="C170" s="79" t="s">
+      <c r="B170" s="94"/>
+      <c r="C170" s="73" t="s">
         <v>322</v>
       </c>
       <c r="D170" s="21" t="s">
@@ -7770,13 +7712,13 @@
       <c r="E170" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F170" s="60">
+      <c r="F170" s="55">
         <v>1</v>
       </c>
-      <c r="G170" s="79" t="s">
+      <c r="G170" s="73" t="s">
         <v>323</v>
       </c>
-      <c r="H170" s="59" t="s">
+      <c r="H170" s="54" t="s">
         <v>324</v>
       </c>
     </row>
@@ -7784,8 +7726,8 @@
       <c r="A171" s="19">
         <v>23</v>
       </c>
-      <c r="B171" s="105"/>
-      <c r="C171" s="77" t="s">
+      <c r="B171" s="94"/>
+      <c r="C171" s="71" t="s">
         <v>120</v>
       </c>
       <c r="D171" s="21" t="s">
@@ -7794,11 +7736,11 @@
       <c r="E171" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F171" s="60"/>
-      <c r="G171" s="68" t="s">
+      <c r="F171" s="55"/>
+      <c r="G171" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="H171" s="59" t="s">
+      <c r="H171" s="54" t="s">
         <v>121</v>
       </c>
     </row>
@@ -7806,8 +7748,8 @@
       <c r="A172" s="19">
         <v>24</v>
       </c>
-      <c r="B172" s="104"/>
-      <c r="C172" s="56" t="s">
+      <c r="B172" s="95"/>
+      <c r="C172" s="51" t="s">
         <v>124</v>
       </c>
       <c r="D172" s="21" t="s">
@@ -7816,25 +7758,25 @@
       <c r="E172" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F172" s="60" t="s">
+      <c r="F172" s="55" t="s">
         <v>317</v>
       </c>
-      <c r="G172" s="56" t="s">
+      <c r="G172" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="H172" s="78" t="s">
+      <c r="H172" s="72" t="s">
         <v>318</v>
       </c>
-      <c r="I172" s="64"/>
+      <c r="I172" s="59"/>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" s="19">
         <v>25</v>
       </c>
-      <c r="B173" s="94" t="s">
+      <c r="B173" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="C173" s="56" t="s">
+      <c r="C173" s="51" t="s">
         <v>122</v>
       </c>
       <c r="D173" s="21" t="s">
@@ -7843,23 +7785,23 @@
       <c r="E173" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F173" s="56" t="s">
+      <c r="F173" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="G173" s="56" t="s">
+      <c r="G173" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H173" s="59" t="s">
+      <c r="H173" s="54" t="s">
         <v>268</v>
       </c>
-      <c r="I173" s="64"/>
+      <c r="I173" s="59"/>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" s="19">
         <v>26</v>
       </c>
-      <c r="B174" s="95"/>
-      <c r="C174" s="68" t="s">
+      <c r="B174" s="109"/>
+      <c r="C174" s="62" t="s">
         <v>262</v>
       </c>
       <c r="D174" s="21" t="s">
@@ -7868,13 +7810,13 @@
       <c r="E174" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F174" s="56" t="s">
+      <c r="F174" s="51" t="s">
         <v>264</v>
       </c>
-      <c r="G174" s="56" t="s">
+      <c r="G174" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H174" s="59" t="s">
+      <c r="H174" s="54" t="s">
         <v>266</v>
       </c>
     </row>
@@ -7882,8 +7824,8 @@
       <c r="A175" s="19">
         <v>27</v>
       </c>
-      <c r="B175" s="95"/>
-      <c r="C175" s="68" t="s">
+      <c r="B175" s="109"/>
+      <c r="C175" s="62" t="s">
         <v>263</v>
       </c>
       <c r="D175" s="21" t="s">
@@ -7892,13 +7834,13 @@
       <c r="E175" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F175" s="56" t="s">
+      <c r="F175" s="51" t="s">
         <v>265</v>
       </c>
-      <c r="G175" s="56" t="s">
+      <c r="G175" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H175" s="67" t="s">
+      <c r="H175" s="61" t="s">
         <v>283</v>
       </c>
     </row>
@@ -7906,8 +7848,8 @@
       <c r="A176" s="19">
         <v>28</v>
       </c>
-      <c r="B176" s="95"/>
-      <c r="C176" s="68" t="s">
+      <c r="B176" s="109"/>
+      <c r="C176" s="62" t="s">
         <v>297</v>
       </c>
       <c r="D176" s="21" t="s">
@@ -7916,20 +7858,20 @@
       <c r="E176" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F176" s="56" t="s">
+      <c r="F176" s="51" t="s">
         <v>265</v>
       </c>
-      <c r="G176" s="56" t="s">
+      <c r="G176" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H176" s="67"/>
+      <c r="H176" s="61"/>
     </row>
     <row r="177" spans="1:8">
       <c r="A177" s="19">
         <v>29</v>
       </c>
-      <c r="B177" s="95"/>
-      <c r="C177" s="68" t="s">
+      <c r="B177" s="109"/>
+      <c r="C177" s="62" t="s">
         <v>284</v>
       </c>
       <c r="D177" s="21" t="s">
@@ -7938,33 +7880,33 @@
       <c r="E177" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F177" s="56" t="s">
+      <c r="F177" s="51" t="s">
         <v>265</v>
       </c>
-      <c r="G177" s="56" t="s">
+      <c r="G177" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H177" s="59"/>
+      <c r="H177" s="54"/>
     </row>
     <row r="178" spans="1:8">
       <c r="A178" s="19">
         <v>30</v>
       </c>
-      <c r="B178" s="95"/>
-      <c r="C178" s="56" t="s">
+      <c r="B178" s="109"/>
+      <c r="C178" s="51" t="s">
         <v>281</v>
       </c>
       <c r="D178" s="21"/>
       <c r="E178" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F178" s="56" t="s">
+      <c r="F178" s="51" t="s">
         <v>282</v>
       </c>
-      <c r="G178" s="56" t="s">
+      <c r="G178" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H178" s="67" t="s">
+      <c r="H178" s="61" t="s">
         <v>289</v>
       </c>
     </row>
@@ -7972,8 +7914,8 @@
       <c r="A179" s="19">
         <v>31</v>
       </c>
-      <c r="B179" s="95"/>
-      <c r="C179" s="70" t="s">
+      <c r="B179" s="109"/>
+      <c r="C179" s="64" t="s">
         <v>291</v>
       </c>
       <c r="D179" s="21" t="s">
@@ -7982,13 +7924,13 @@
       <c r="E179" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F179" s="70" t="s">
+      <c r="F179" s="64" t="s">
         <v>288</v>
       </c>
-      <c r="G179" s="72" t="s">
+      <c r="G179" s="66" t="s">
         <v>301</v>
       </c>
-      <c r="H179" s="67" t="s">
+      <c r="H179" s="61" t="s">
         <v>290</v>
       </c>
     </row>
@@ -7996,21 +7938,21 @@
       <c r="A180" s="19">
         <v>32</v>
       </c>
-      <c r="B180" s="95"/>
-      <c r="C180" s="56" t="s">
+      <c r="B180" s="109"/>
+      <c r="C180" s="51" t="s">
         <v>279</v>
       </c>
-      <c r="D180" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="E180" s="56"/>
-      <c r="F180" s="56" t="s">
+      <c r="D180" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E180" s="51"/>
+      <c r="F180" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="G180" s="56" t="s">
+      <c r="G180" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="H180" s="59" t="s">
+      <c r="H180" s="54" t="s">
         <v>280</v>
       </c>
     </row>
@@ -8018,23 +7960,23 @@
       <c r="A181" s="19">
         <v>33</v>
       </c>
-      <c r="B181" s="95"/>
-      <c r="C181" s="68" t="s">
+      <c r="B181" s="109"/>
+      <c r="C181" s="62" t="s">
         <v>287</v>
       </c>
-      <c r="D181" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="E181" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="F181" s="70" t="s">
+      <c r="D181" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E181" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="F181" s="64" t="s">
         <v>300</v>
       </c>
-      <c r="G181" s="70" t="s">
+      <c r="G181" s="64" t="s">
         <v>298</v>
       </c>
-      <c r="H181" s="71" t="s">
+      <c r="H181" s="65" t="s">
         <v>299</v>
       </c>
     </row>
@@ -8042,8 +7984,8 @@
       <c r="A182" s="19">
         <v>34</v>
       </c>
-      <c r="B182" s="95"/>
-      <c r="C182" s="56" t="s">
+      <c r="B182" s="109"/>
+      <c r="C182" s="51" t="s">
         <v>223</v>
       </c>
       <c r="D182" s="21" t="s">
@@ -8053,10 +7995,10 @@
         <v>89</v>
       </c>
       <c r="F182" s="21"/>
-      <c r="G182" s="56" t="s">
+      <c r="G182" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H182" s="59" t="s">
+      <c r="H182" s="54" t="s">
         <v>286</v>
       </c>
     </row>
@@ -8064,8 +8006,8 @@
       <c r="A183" s="19">
         <v>35</v>
       </c>
-      <c r="B183" s="102"/>
-      <c r="C183" s="56" t="s">
+      <c r="B183" s="105"/>
+      <c r="C183" s="51" t="s">
         <v>124</v>
       </c>
       <c r="D183" s="21" t="s">
@@ -8078,7 +8020,7 @@
       <c r="G183" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="H183" s="67" t="s">
+      <c r="H183" s="61" t="s">
         <v>319</v>
       </c>
     </row>
@@ -8086,7 +8028,7 @@
       <c r="A184" s="19">
         <v>36</v>
       </c>
-      <c r="B184" s="105" t="s">
+      <c r="B184" s="94" t="s">
         <v>6</v>
       </c>
       <c r="C184" s="21" t="s">
@@ -8098,13 +8040,13 @@
       <c r="E184" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F184" s="56" t="s">
+      <c r="F184" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="G184" s="56" t="s">
+      <c r="G184" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="H184" s="59" t="s">
+      <c r="H184" s="54" t="s">
         <v>274</v>
       </c>
     </row>
@@ -8112,8 +8054,8 @@
       <c r="A185" s="19">
         <v>37</v>
       </c>
-      <c r="B185" s="104"/>
-      <c r="C185" s="56" t="s">
+      <c r="B185" s="95"/>
+      <c r="C185" s="51" t="s">
         <v>269</v>
       </c>
       <c r="D185" s="21" t="s">
@@ -8122,13 +8064,13 @@
       <c r="E185" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F185" s="56" t="s">
+      <c r="F185" s="51" t="s">
         <v>270</v>
       </c>
-      <c r="G185" s="68" t="s">
+      <c r="G185" s="62" t="s">
         <v>271</v>
       </c>
-      <c r="H185" s="59" t="s">
+      <c r="H185" s="54" t="s">
         <v>272</v>
       </c>
     </row>
@@ -8136,8 +8078,8 @@
       <c r="A186" s="19">
         <v>38</v>
       </c>
-      <c r="B186" s="104"/>
-      <c r="C186" s="56" t="s">
+      <c r="B186" s="95"/>
+      <c r="C186" s="51" t="s">
         <v>129</v>
       </c>
       <c r="D186" s="21" t="s">
@@ -8156,7 +8098,7 @@
       <c r="A187" s="19">
         <v>39</v>
       </c>
-      <c r="B187" s="104"/>
+      <c r="B187" s="95"/>
       <c r="C187" s="21" t="s">
         <v>130</v>
       </c>
@@ -8169,10 +8111,10 @@
       <c r="F187" s="21">
         <v>20.03</v>
       </c>
-      <c r="G187" s="56">
+      <c r="G187" s="51">
         <v>20.03</v>
       </c>
-      <c r="H187" s="59" t="s">
+      <c r="H187" s="54" t="s">
         <v>275</v>
       </c>
     </row>
@@ -8180,7 +8122,7 @@
       <c r="A188" s="19">
         <v>40</v>
       </c>
-      <c r="B188" s="104"/>
+      <c r="B188" s="95"/>
       <c r="C188" s="21" t="s">
         <v>131</v>
       </c>
@@ -8202,7 +8144,7 @@
       <c r="A189" s="19">
         <v>41</v>
       </c>
-      <c r="B189" s="104"/>
+      <c r="B189" s="95"/>
       <c r="C189" s="21" t="s">
         <v>132</v>
       </c>
@@ -8222,7 +8164,7 @@
       <c r="A190" s="19">
         <v>42</v>
       </c>
-      <c r="B190" s="104"/>
+      <c r="B190" s="95"/>
       <c r="C190" s="21" t="s">
         <v>133</v>
       </c>
@@ -8242,7 +8184,7 @@
       <c r="A191" s="19">
         <v>43</v>
       </c>
-      <c r="B191" s="104"/>
+      <c r="B191" s="95"/>
       <c r="C191" s="21" t="s">
         <v>43</v>
       </c>
@@ -8262,7 +8204,7 @@
       <c r="A192" s="19">
         <v>44</v>
       </c>
-      <c r="B192" s="105" t="s">
+      <c r="B192" s="94" t="s">
         <v>7</v>
       </c>
       <c r="C192" s="21" t="s">
@@ -8274,10 +8216,10 @@
       <c r="E192" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F192" s="56" t="s">
+      <c r="F192" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="G192" s="63" t="s">
+      <c r="G192" s="58" t="s">
         <v>278</v>
       </c>
       <c r="H192" s="11"/>
@@ -8286,8 +8228,8 @@
       <c r="A193" s="19">
         <v>45</v>
       </c>
-      <c r="B193" s="104"/>
-      <c r="C193" s="56" t="s">
+      <c r="B193" s="95"/>
+      <c r="C193" s="51" t="s">
         <v>135</v>
       </c>
       <c r="D193" s="21" t="s">
@@ -8296,10 +8238,10 @@
       <c r="E193" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F193" s="56" t="s">
+      <c r="F193" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="G193" s="56" t="s">
+      <c r="G193" s="51" t="s">
         <v>137</v>
       </c>
       <c r="H193" s="11"/>
@@ -8308,8 +8250,8 @@
       <c r="A194" s="19">
         <v>46</v>
       </c>
-      <c r="B194" s="104"/>
-      <c r="C194" s="56" t="s">
+      <c r="B194" s="95"/>
+      <c r="C194" s="51" t="s">
         <v>247</v>
       </c>
       <c r="D194" s="21" t="s">
@@ -8318,10 +8260,10 @@
       <c r="E194" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F194" s="56" t="s">
+      <c r="F194" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="G194" s="56" t="s">
+      <c r="G194" s="51" t="s">
         <v>248</v>
       </c>
       <c r="H194" s="11"/>
@@ -8330,8 +8272,8 @@
       <c r="A195" s="19">
         <v>47</v>
       </c>
-      <c r="B195" s="104"/>
-      <c r="C195" s="56" t="s">
+      <c r="B195" s="95"/>
+      <c r="C195" s="51" t="s">
         <v>138</v>
       </c>
       <c r="D195" s="21" t="s">
@@ -8340,10 +8282,10 @@
       <c r="E195" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F195" s="56" t="s">
+      <c r="F195" s="51" t="s">
         <v>243</v>
       </c>
-      <c r="G195" s="56" t="s">
+      <c r="G195" s="51" t="s">
         <v>243</v>
       </c>
       <c r="H195" s="11"/>
@@ -8352,8 +8294,8 @@
       <c r="A196" s="19">
         <v>48</v>
       </c>
-      <c r="B196" s="104"/>
-      <c r="C196" s="56" t="s">
+      <c r="B196" s="95"/>
+      <c r="C196" s="51" t="s">
         <v>245</v>
       </c>
       <c r="D196" s="21" t="s">
@@ -8362,10 +8304,10 @@
       <c r="E196" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F196" s="56">
+      <c r="F196" s="51">
         <v>64</v>
       </c>
-      <c r="G196" s="56" t="s">
+      <c r="G196" s="51" t="s">
         <v>244</v>
       </c>
       <c r="H196" s="11"/>
@@ -8374,8 +8316,8 @@
       <c r="A197" s="19">
         <v>49</v>
       </c>
-      <c r="B197" s="104"/>
-      <c r="C197" s="56" t="s">
+      <c r="B197" s="95"/>
+      <c r="C197" s="51" t="s">
         <v>246</v>
       </c>
       <c r="D197" s="21" t="s">
@@ -8384,10 +8326,10 @@
       <c r="E197" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F197" s="56">
+      <c r="F197" s="51">
         <v>7.9</v>
       </c>
-      <c r="G197" s="56" t="s">
+      <c r="G197" s="51" t="s">
         <v>249</v>
       </c>
       <c r="H197" s="11"/>
@@ -8396,21 +8338,21 @@
       <c r="A198" s="19">
         <v>50</v>
       </c>
-      <c r="B198" s="104"/>
-      <c r="C198" s="56" t="s">
+      <c r="B198" s="95"/>
+      <c r="C198" s="51" t="s">
         <v>302</v>
       </c>
       <c r="D198" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E198" s="21"/>
-      <c r="F198" s="56">
+      <c r="F198" s="51">
         <v>50</v>
       </c>
-      <c r="G198" s="56" t="s">
+      <c r="G198" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="H198" s="59" t="s">
+      <c r="H198" s="54" t="s">
         <v>307</v>
       </c>
     </row>
@@ -8418,21 +8360,21 @@
       <c r="A199" s="19">
         <v>51</v>
       </c>
-      <c r="B199" s="104"/>
-      <c r="C199" s="56" t="s">
+      <c r="B199" s="95"/>
+      <c r="C199" s="51" t="s">
         <v>303</v>
       </c>
       <c r="D199" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E199" s="21"/>
-      <c r="F199" s="56">
+      <c r="F199" s="51">
         <v>50</v>
       </c>
-      <c r="G199" s="56" t="s">
+      <c r="G199" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="H199" s="59" t="s">
+      <c r="H199" s="54" t="s">
         <v>308</v>
       </c>
     </row>
@@ -8440,8 +8382,8 @@
       <c r="A200" s="19">
         <v>52</v>
       </c>
-      <c r="B200" s="104"/>
-      <c r="C200" s="56" t="s">
+      <c r="B200" s="95"/>
+      <c r="C200" s="51" t="s">
         <v>304</v>
       </c>
       <c r="D200" s="21" t="s">
@@ -8451,10 +8393,10 @@
       <c r="F200" s="21">
         <v>10</v>
       </c>
-      <c r="G200" s="56" t="s">
+      <c r="G200" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="H200" s="59" t="s">
+      <c r="H200" s="54" t="s">
         <v>309</v>
       </c>
     </row>
@@ -8462,7 +8404,7 @@
       <c r="A201" s="19">
         <v>53</v>
       </c>
-      <c r="B201" s="94" t="s">
+      <c r="B201" s="111" t="s">
         <v>8</v>
       </c>
       <c r="C201" s="21" t="s">
@@ -8488,7 +8430,7 @@
       <c r="A202" s="19">
         <v>54</v>
       </c>
-      <c r="B202" s="95"/>
+      <c r="B202" s="109"/>
       <c r="C202" s="20" t="s">
         <v>142</v>
       </c>
@@ -8512,8 +8454,8 @@
       <c r="A203" s="19">
         <v>55</v>
       </c>
-      <c r="B203" s="96"/>
-      <c r="C203" s="58" t="s">
+      <c r="B203" s="110"/>
+      <c r="C203" s="53" t="s">
         <v>250</v>
       </c>
       <c r="D203" s="20" t="s">
@@ -8522,7 +8464,7 @@
       <c r="E203" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="F203" s="58" t="s">
+      <c r="F203" s="53" t="s">
         <v>251</v>
       </c>
       <c r="G203" s="20" t="s">
@@ -8536,10 +8478,10 @@
       <c r="A204" s="16">
         <v>56</v>
       </c>
-      <c r="B204" s="97" t="s">
+      <c r="B204" s="112" t="s">
         <v>76</v>
       </c>
-      <c r="C204" s="57" t="s">
+      <c r="C204" s="52" t="s">
         <v>144</v>
       </c>
       <c r="D204" s="17" t="s">
@@ -8551,27 +8493,27 @@
       <c r="F204" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="G204" s="57" t="s">
+      <c r="G204" s="52" t="s">
         <v>146</v>
       </c>
       <c r="H204" s="10"/>
     </row>
     <row r="205" spans="1:8">
-      <c r="A205" s="75">
+      <c r="A205" s="69">
         <v>57</v>
       </c>
-      <c r="B205" s="98"/>
-      <c r="C205" s="76" t="s">
+      <c r="B205" s="113"/>
+      <c r="C205" s="70" t="s">
         <v>313</v>
       </c>
-      <c r="D205" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="E205" s="74"/>
-      <c r="F205" s="74" t="s">
+      <c r="D205" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="E205" s="68"/>
+      <c r="F205" s="68" t="s">
         <v>152</v>
       </c>
-      <c r="G205" s="73" t="s">
+      <c r="G205" s="67" t="s">
         <v>314</v>
       </c>
       <c r="H205" s="36" t="s">
@@ -8579,11 +8521,11 @@
       </c>
     </row>
     <row r="206" spans="1:8">
-      <c r="A206" s="75">
+      <c r="A206" s="69">
         <v>58</v>
       </c>
-      <c r="B206" s="99"/>
-      <c r="C206" s="56" t="s">
+      <c r="B206" s="114"/>
+      <c r="C206" s="51" t="s">
         <v>147</v>
       </c>
       <c r="D206" s="21" t="s">
@@ -8595,17 +8537,17 @@
       <c r="F206" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="G206" s="58" t="s">
+      <c r="G206" s="53" t="s">
         <v>149</v>
       </c>
       <c r="H206" s="11"/>
     </row>
     <row r="207" spans="1:8">
-      <c r="A207" s="75">
+      <c r="A207" s="69">
         <v>59</v>
       </c>
-      <c r="B207" s="100"/>
-      <c r="C207" s="58" t="s">
+      <c r="B207" s="115"/>
+      <c r="C207" s="53" t="s">
         <v>150</v>
       </c>
       <c r="D207" s="21" t="s">
@@ -8623,11 +8565,11 @@
       <c r="H207" s="22"/>
     </row>
     <row r="208" spans="1:8">
-      <c r="A208" s="75">
+      <c r="A208" s="69">
         <v>60</v>
       </c>
-      <c r="B208" s="100"/>
-      <c r="C208" s="58" t="s">
+      <c r="B208" s="115"/>
+      <c r="C208" s="53" t="s">
         <v>151</v>
       </c>
       <c r="D208" s="20" t="s">
@@ -8639,17 +8581,17 @@
       <c r="F208" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="G208" s="58" t="s">
+      <c r="G208" s="53" t="s">
         <v>153</v>
       </c>
       <c r="H208" s="22"/>
     </row>
     <row r="209" spans="1:8">
-      <c r="A209" s="75">
+      <c r="A209" s="69">
         <v>61</v>
       </c>
-      <c r="B209" s="100"/>
-      <c r="C209" s="58" t="s">
+      <c r="B209" s="115"/>
+      <c r="C209" s="53" t="s">
         <v>154</v>
       </c>
       <c r="D209" s="20" t="s">
@@ -8659,17 +8601,17 @@
         <v>89</v>
       </c>
       <c r="F209" s="20"/>
-      <c r="G209" s="60" t="s">
+      <c r="G209" s="55" t="s">
         <v>235</v>
       </c>
       <c r="H209" s="22"/>
     </row>
     <row r="210" spans="1:8">
-      <c r="A210" s="75">
+      <c r="A210" s="69">
         <v>62</v>
       </c>
-      <c r="B210" s="100"/>
-      <c r="C210" s="58" t="s">
+      <c r="B210" s="115"/>
+      <c r="C210" s="53" t="s">
         <v>229</v>
       </c>
       <c r="D210" s="20" t="s">
@@ -8679,7 +8621,7 @@
       <c r="F210" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="G210" s="58" t="s">
+      <c r="G210" s="53" t="s">
         <v>231</v>
       </c>
       <c r="H210" s="22" t="s">
@@ -8687,11 +8629,11 @@
       </c>
     </row>
     <row r="211" spans="1:8">
-      <c r="A211" s="75">
+      <c r="A211" s="69">
         <v>63</v>
       </c>
-      <c r="B211" s="100"/>
-      <c r="C211" s="58" t="s">
+      <c r="B211" s="115"/>
+      <c r="C211" s="53" t="s">
         <v>233</v>
       </c>
       <c r="D211" s="20" t="s">
@@ -8701,7 +8643,7 @@
       <c r="F211" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="G211" s="58" t="s">
+      <c r="G211" s="53" t="s">
         <v>149</v>
       </c>
       <c r="H211" s="22" t="s">
@@ -8712,7 +8654,7 @@
       <c r="A212" s="23">
         <v>64</v>
       </c>
-      <c r="B212" s="101"/>
+      <c r="B212" s="99"/>
       <c r="C212" s="24" t="s">
         <v>320</v>
       </c>
@@ -8744,22 +8686,22 @@
       </c>
     </row>
     <row r="215" spans="1:8">
-      <c r="B215" s="64" t="s">
+      <c r="B215" s="59" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="216" spans="1:8">
-      <c r="B216" s="64" t="s">
+      <c r="B216" s="59" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="217" spans="1:8">
-      <c r="B217" s="66" t="s">
+      <c r="B217" s="60" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="218" spans="1:8">
-      <c r="B218" s="64" t="s">
+      <c r="B218" s="59" t="s">
         <v>277</v>
       </c>
     </row>
@@ -8778,11 +8720,11 @@
       <c r="B229" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C229" s="128" t="s">
+      <c r="C229" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="D229" s="128"/>
-      <c r="E229" s="128"/>
+      <c r="D229" s="85"/>
+      <c r="E229" s="85"/>
       <c r="F229" s="32" t="s">
         <v>162</v>
       </c>
@@ -8791,32 +8733,32 @@
       </c>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="109" t="s">
+      <c r="A230" s="106" t="s">
         <v>164</v>
       </c>
-      <c r="B230" s="102" t="s">
+      <c r="B230" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="C230" s="129" t="s">
+      <c r="C230" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="D230" s="130"/>
-      <c r="E230" s="130"/>
-      <c r="F230" s="74" t="s">
+      <c r="D230" s="87"/>
+      <c r="E230" s="87"/>
+      <c r="F230" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="G230" s="83" t="s">
+      <c r="G230" s="77" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="110"/>
-      <c r="B231" s="103"/>
-      <c r="C231" s="120" t="s">
+      <c r="A231" s="107"/>
+      <c r="B231" s="116"/>
+      <c r="C231" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="D231" s="131"/>
-      <c r="E231" s="131"/>
+      <c r="D231" s="89"/>
+      <c r="E231" s="89"/>
       <c r="F231" s="20" t="s">
         <v>169</v>
       </c>
@@ -8825,15 +8767,15 @@
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="110"/>
-      <c r="B232" s="104" t="s">
+      <c r="A232" s="107"/>
+      <c r="B232" s="95" t="s">
         <v>170</v>
       </c>
-      <c r="C232" s="124" t="s">
+      <c r="C232" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="D232" s="124"/>
-      <c r="E232" s="124"/>
+      <c r="D232" s="90"/>
+      <c r="E232" s="90"/>
       <c r="F232" s="21" t="s">
         <v>167</v>
       </c>
@@ -8842,13 +8784,13 @@
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="110"/>
-      <c r="B233" s="104"/>
-      <c r="C233" s="120" t="s">
+      <c r="A233" s="107"/>
+      <c r="B233" s="95"/>
+      <c r="C233" s="88" t="s">
         <v>171</v>
       </c>
-      <c r="D233" s="120"/>
-      <c r="E233" s="120"/>
+      <c r="D233" s="88"/>
+      <c r="E233" s="88"/>
       <c r="F233" s="21" t="s">
         <v>169</v>
       </c>
@@ -8857,15 +8799,15 @@
       </c>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="110"/>
-      <c r="B234" s="103" t="s">
+      <c r="A234" s="107"/>
+      <c r="B234" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="C234" s="121" t="s">
+      <c r="C234" s="91" t="s">
         <v>166</v>
       </c>
-      <c r="D234" s="122"/>
-      <c r="E234" s="123"/>
+      <c r="D234" s="92"/>
+      <c r="E234" s="93"/>
       <c r="F234" s="21" t="s">
         <v>167</v>
       </c>
@@ -8874,13 +8816,13 @@
       </c>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="110"/>
-      <c r="B235" s="102"/>
-      <c r="C235" s="121" t="s">
+      <c r="A235" s="107"/>
+      <c r="B235" s="105"/>
+      <c r="C235" s="91" t="s">
         <v>166</v>
       </c>
-      <c r="D235" s="122"/>
-      <c r="E235" s="123"/>
+      <c r="D235" s="92"/>
+      <c r="E235" s="93"/>
       <c r="F235" s="21" t="s">
         <v>169</v>
       </c>
@@ -8889,15 +8831,15 @@
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="110"/>
-      <c r="B236" s="104" t="s">
+      <c r="A236" s="107"/>
+      <c r="B236" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="C236" s="124" t="s">
+      <c r="C236" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="D236" s="124"/>
-      <c r="E236" s="124"/>
+      <c r="D236" s="90"/>
+      <c r="E236" s="90"/>
       <c r="F236" s="21" t="s">
         <v>167</v>
       </c>
@@ -8906,13 +8848,13 @@
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="110"/>
-      <c r="B237" s="104"/>
-      <c r="C237" s="124" t="s">
+      <c r="A237" s="107"/>
+      <c r="B237" s="95"/>
+      <c r="C237" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="D237" s="124"/>
-      <c r="E237" s="124"/>
+      <c r="D237" s="90"/>
+      <c r="E237" s="90"/>
       <c r="F237" s="21" t="s">
         <v>169</v>
       </c>
@@ -8921,17 +8863,17 @@
       </c>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="110" t="s">
+      <c r="A238" s="107" t="s">
         <v>175</v>
       </c>
-      <c r="B238" s="104" t="s">
+      <c r="B238" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="C238" s="105" t="s">
+      <c r="C238" s="94" t="s">
         <v>177</v>
       </c>
-      <c r="D238" s="104"/>
-      <c r="E238" s="104"/>
+      <c r="D238" s="95"/>
+      <c r="E238" s="95"/>
       <c r="F238" s="21" t="s">
         <v>167</v>
       </c>
@@ -8940,13 +8882,13 @@
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="110"/>
-      <c r="B239" s="104"/>
-      <c r="C239" s="104" t="s">
+      <c r="A239" s="107"/>
+      <c r="B239" s="95"/>
+      <c r="C239" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="D239" s="104"/>
-      <c r="E239" s="104"/>
+      <c r="D239" s="95"/>
+      <c r="E239" s="95"/>
       <c r="F239" s="21" t="s">
         <v>169</v>
       </c>
@@ -8955,15 +8897,15 @@
       </c>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="110"/>
-      <c r="B240" s="104" t="s">
+      <c r="A240" s="107"/>
+      <c r="B240" s="95" t="s">
         <v>180</v>
       </c>
-      <c r="C240" s="104" t="s">
+      <c r="C240" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="D240" s="104"/>
-      <c r="E240" s="104"/>
+      <c r="D240" s="95"/>
+      <c r="E240" s="95"/>
       <c r="F240" s="21" t="s">
         <v>167</v>
       </c>
@@ -8972,13 +8914,13 @@
       </c>
     </row>
     <row r="241" spans="1:7">
-      <c r="A241" s="110"/>
-      <c r="B241" s="104"/>
-      <c r="C241" s="104" t="s">
+      <c r="A241" s="107"/>
+      <c r="B241" s="95"/>
+      <c r="C241" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="D241" s="104"/>
-      <c r="E241" s="104"/>
+      <c r="D241" s="95"/>
+      <c r="E241" s="95"/>
       <c r="F241" s="21" t="s">
         <v>169</v>
       </c>
@@ -8987,17 +8929,17 @@
       </c>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="110" t="s">
+      <c r="A242" s="107" t="s">
         <v>183</v>
       </c>
-      <c r="B242" s="104" t="s">
+      <c r="B242" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="C242" s="105" t="s">
+      <c r="C242" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D242" s="104"/>
-      <c r="E242" s="104"/>
+      <c r="D242" s="95"/>
+      <c r="E242" s="95"/>
       <c r="F242" s="21" t="s">
         <v>167</v>
       </c>
@@ -9006,13 +8948,13 @@
       </c>
     </row>
     <row r="243" spans="1:7">
-      <c r="A243" s="110"/>
-      <c r="B243" s="104"/>
-      <c r="C243" s="104" t="s">
+      <c r="A243" s="107"/>
+      <c r="B243" s="95"/>
+      <c r="C243" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="D243" s="104"/>
-      <c r="E243" s="104"/>
+      <c r="D243" s="95"/>
+      <c r="E243" s="95"/>
       <c r="F243" s="21" t="s">
         <v>169</v>
       </c>
@@ -9021,15 +8963,15 @@
       </c>
     </row>
     <row r="244" spans="1:7">
-      <c r="A244" s="110"/>
-      <c r="B244" s="104" t="s">
+      <c r="A244" s="107"/>
+      <c r="B244" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="C244" s="105" t="s">
+      <c r="C244" s="94" t="s">
         <v>188</v>
       </c>
-      <c r="D244" s="104"/>
-      <c r="E244" s="104"/>
+      <c r="D244" s="95"/>
+      <c r="E244" s="95"/>
       <c r="F244" s="21" t="s">
         <v>167</v>
       </c>
@@ -9038,13 +8980,13 @@
       </c>
     </row>
     <row r="245" spans="1:7">
-      <c r="A245" s="111"/>
-      <c r="B245" s="112"/>
-      <c r="C245" s="112" t="s">
+      <c r="A245" s="108"/>
+      <c r="B245" s="100"/>
+      <c r="C245" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="D245" s="112"/>
-      <c r="E245" s="112"/>
+      <c r="D245" s="100"/>
+      <c r="E245" s="100"/>
       <c r="F245" s="24" t="s">
         <v>169</v>
       </c>
@@ -9066,12 +9008,12 @@
       <c r="A250" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="B250" s="118" t="s">
+      <c r="B250" s="103" t="s">
         <v>193</v>
       </c>
-      <c r="C250" s="118"/>
-      <c r="D250" s="118"/>
-      <c r="E250" s="118"/>
+      <c r="C250" s="103"/>
+      <c r="D250" s="103"/>
+      <c r="E250" s="103"/>
       <c r="F250" s="32" t="s">
         <v>194</v>
       </c>
@@ -9083,12 +9025,12 @@
       <c r="A251" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="B251" s="119" t="s">
+      <c r="B251" s="104" t="s">
         <v>197</v>
       </c>
-      <c r="C251" s="102"/>
-      <c r="D251" s="102"/>
-      <c r="E251" s="102"/>
+      <c r="C251" s="105"/>
+      <c r="D251" s="105"/>
+      <c r="E251" s="105"/>
       <c r="F251" s="35" t="s">
         <v>74</v>
       </c>
@@ -9100,12 +9042,12 @@
       <c r="A252" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B252" s="114" t="s">
+      <c r="B252" s="96" t="s">
         <v>199</v>
       </c>
-      <c r="C252" s="115"/>
-      <c r="D252" s="115"/>
-      <c r="E252" s="116"/>
+      <c r="C252" s="97"/>
+      <c r="D252" s="97"/>
+      <c r="E252" s="98"/>
       <c r="F252" s="9" t="s">
         <v>168</v>
       </c>
@@ -9117,12 +9059,12 @@
       <c r="A253" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B253" s="114" t="s">
+      <c r="B253" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="C253" s="115"/>
-      <c r="D253" s="115"/>
-      <c r="E253" s="116"/>
+      <c r="C253" s="97"/>
+      <c r="D253" s="97"/>
+      <c r="E253" s="98"/>
       <c r="F253" s="13" t="s">
         <v>168</v>
       </c>
@@ -9134,12 +9076,12 @@
       <c r="A254" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B254" s="101" t="s">
+      <c r="B254" s="99" t="s">
         <v>203</v>
       </c>
-      <c r="C254" s="112"/>
-      <c r="D254" s="112"/>
-      <c r="E254" s="112"/>
+      <c r="C254" s="100"/>
+      <c r="D254" s="100"/>
+      <c r="E254" s="100"/>
       <c r="F254" s="15" t="s">
         <v>168</v>
       </c>
@@ -9155,7 +9097,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" ht="15.75" thickBot="1">
       <c r="A258" s="4" t="s">
         <v>205</v>
       </c>
@@ -9184,11 +9126,11 @@
       <c r="C259" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="D259" s="117" t="s">
+      <c r="D259" s="101" t="s">
         <v>209</v>
       </c>
-      <c r="E259" s="117"/>
-      <c r="F259" s="117"/>
+      <c r="E259" s="101"/>
+      <c r="F259" s="101"/>
       <c r="G259" s="18"/>
     </row>
     <row r="260" spans="1:7">
@@ -9201,11 +9143,11 @@
       <c r="C260" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D260" s="113" t="s">
+      <c r="D260" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="E260" s="113"/>
-      <c r="F260" s="113"/>
+      <c r="E260" s="102"/>
+      <c r="F260" s="102"/>
       <c r="G260" s="28"/>
     </row>
     <row r="261" spans="1:7">
@@ -9218,11 +9160,11 @@
       <c r="C261" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D261" s="113" t="s">
+      <c r="D261" s="102" t="s">
         <v>211</v>
       </c>
-      <c r="E261" s="113"/>
-      <c r="F261" s="113"/>
+      <c r="E261" s="102"/>
+      <c r="F261" s="102"/>
       <c r="G261" s="28"/>
     </row>
     <row r="262" spans="1:7">
@@ -9235,11 +9177,11 @@
       <c r="C262" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D262" s="113" t="s">
+      <c r="D262" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="E262" s="113"/>
-      <c r="F262" s="113"/>
+      <c r="E262" s="102"/>
+      <c r="F262" s="102"/>
       <c r="G262" s="28"/>
     </row>
     <row r="263" spans="1:7">
@@ -9252,11 +9194,11 @@
       <c r="C263" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D263" s="113" t="s">
+      <c r="D263" s="102" t="s">
         <v>213</v>
       </c>
-      <c r="E263" s="113"/>
-      <c r="F263" s="113"/>
+      <c r="E263" s="102"/>
+      <c r="F263" s="102"/>
       <c r="G263" s="28"/>
     </row>
     <row r="264" spans="1:7">
@@ -9269,338 +9211,355 @@
       <c r="C264" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D264" s="113" t="s">
+      <c r="D264" s="102" t="s">
         <v>214</v>
       </c>
-      <c r="E264" s="113"/>
-      <c r="F264" s="113"/>
+      <c r="E264" s="102"/>
+      <c r="F264" s="102"/>
       <c r="G264" s="28"/>
     </row>
     <row r="265" spans="1:7">
-      <c r="A265" s="44">
+      <c r="A265" s="42">
         <v>43248</v>
       </c>
-      <c r="B265" s="45">
+      <c r="B265" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C265" s="20" t="s">
+      <c r="C265" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D265" s="106" t="s">
+      <c r="D265" s="102" t="s">
         <v>215</v>
       </c>
-      <c r="E265" s="107"/>
-      <c r="F265" s="108"/>
-      <c r="G265" s="29"/>
+      <c r="E265" s="102"/>
+      <c r="F265" s="102"/>
+      <c r="G265" s="28"/>
     </row>
     <row r="266" spans="1:7">
-      <c r="A266" s="44">
+      <c r="A266" s="42">
         <v>43339</v>
       </c>
-      <c r="B266" s="45">
+      <c r="B266" s="43">
         <v>1.1100000000000001</v>
       </c>
-      <c r="C266" s="20" t="s">
+      <c r="C266" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D266" s="106" t="s">
+      <c r="D266" s="102" t="s">
         <v>216</v>
       </c>
-      <c r="E266" s="107"/>
-      <c r="F266" s="108"/>
-      <c r="G266" s="29"/>
+      <c r="E266" s="102"/>
+      <c r="F266" s="102"/>
+      <c r="G266" s="28"/>
     </row>
     <row r="267" spans="1:7">
-      <c r="A267" s="44">
+      <c r="A267" s="42">
         <v>43542</v>
       </c>
-      <c r="B267" s="45">
+      <c r="B267" s="43">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C267" s="20" t="s">
+      <c r="C267" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D267" s="106" t="s">
+      <c r="D267" s="102" t="s">
         <v>217</v>
       </c>
-      <c r="E267" s="107"/>
-      <c r="F267" s="108"/>
-      <c r="G267" s="29"/>
+      <c r="E267" s="102"/>
+      <c r="F267" s="102"/>
+      <c r="G267" s="28"/>
     </row>
     <row r="268" spans="1:7">
-      <c r="A268" s="44">
+      <c r="A268" s="42">
         <v>43599</v>
       </c>
-      <c r="B268" s="45">
+      <c r="B268" s="43">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C268" s="20" t="s">
+      <c r="C268" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D268" s="46" t="s">
+      <c r="D268" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="E268" s="47"/>
-      <c r="F268" s="48"/>
-      <c r="G268" s="29"/>
+      <c r="E268" s="9"/>
+      <c r="F268" s="9"/>
+      <c r="G268" s="28"/>
     </row>
     <row r="269" spans="1:7">
-      <c r="A269" s="44">
+      <c r="A269" s="42">
         <v>43643</v>
       </c>
-      <c r="B269" s="45">
+      <c r="B269" s="43">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C269" s="20" t="s">
+      <c r="C269" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D269" s="46" t="s">
+      <c r="D269" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="E269" s="47"/>
-      <c r="F269" s="48"/>
-      <c r="G269" s="29"/>
+      <c r="E269" s="9"/>
+      <c r="F269" s="9"/>
+      <c r="G269" s="28"/>
     </row>
     <row r="270" spans="1:7">
-      <c r="A270" s="44">
+      <c r="A270" s="42">
         <v>43894</v>
       </c>
-      <c r="B270" s="45">
+      <c r="B270" s="43">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C270" s="20" t="s">
+      <c r="C270" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D270" s="46" t="s">
+      <c r="D270" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="E270" s="47"/>
-      <c r="F270" s="48"/>
-      <c r="G270" s="29"/>
+      <c r="E270" s="9"/>
+      <c r="F270" s="9"/>
+      <c r="G270" s="28"/>
     </row>
     <row r="271" spans="1:7">
-      <c r="A271" s="44">
+      <c r="A271" s="42">
         <v>44017</v>
       </c>
-      <c r="B271" s="45">
+      <c r="B271" s="43">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C271" s="20" t="s">
+      <c r="C271" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D271" s="46" t="s">
+      <c r="D271" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E271" s="47"/>
-      <c r="F271" s="48"/>
-      <c r="G271" s="29"/>
+      <c r="E271" s="9"/>
+      <c r="F271" s="9"/>
+      <c r="G271" s="28"/>
     </row>
     <row r="272" spans="1:7">
-      <c r="A272" s="44">
+      <c r="A272" s="42">
         <v>44118</v>
       </c>
-      <c r="B272" s="45">
+      <c r="B272" s="43">
         <v>1.17</v>
       </c>
-      <c r="C272" s="20" t="s">
+      <c r="C272" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D272" s="46" t="s">
+      <c r="D272" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="E272" s="47"/>
-      <c r="F272" s="48"/>
-      <c r="G272" s="29"/>
+      <c r="E272" s="9"/>
+      <c r="F272" s="9"/>
+      <c r="G272" s="28"/>
     </row>
     <row r="273" spans="1:7">
-      <c r="A273" s="44">
+      <c r="A273" s="42">
         <v>44209</v>
       </c>
-      <c r="B273" s="45">
+      <c r="B273" s="43">
         <v>1.18</v>
       </c>
-      <c r="C273" s="20" t="s">
+      <c r="C273" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D273" s="65" t="s">
+      <c r="D273" s="57" t="s">
         <v>239</v>
       </c>
-      <c r="E273" s="47"/>
-      <c r="F273" s="48"/>
-      <c r="G273" s="29"/>
+      <c r="E273" s="9"/>
+      <c r="F273" s="9"/>
+      <c r="G273" s="28"/>
     </row>
     <row r="274" spans="1:7">
-      <c r="A274" s="44">
+      <c r="A274" s="42">
         <v>44258</v>
       </c>
-      <c r="B274" s="45">
+      <c r="B274" s="43">
         <v>1.19</v>
       </c>
-      <c r="C274" s="20" t="s">
+      <c r="C274" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D274" s="46" t="s">
+      <c r="D274" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="E274" s="47"/>
-      <c r="F274" s="48"/>
-      <c r="G274" s="29"/>
+      <c r="E274" s="9"/>
+      <c r="F274" s="9"/>
+      <c r="G274" s="28"/>
     </row>
     <row r="275" spans="1:7">
-      <c r="A275" s="44">
+      <c r="A275" s="42">
         <v>44357</v>
       </c>
-      <c r="B275" s="45">
+      <c r="B275" s="43">
         <v>1.2</v>
       </c>
-      <c r="C275" s="20" t="s">
+      <c r="C275" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D275" s="46" t="s">
+      <c r="D275" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E275" s="47"/>
-      <c r="F275" s="48"/>
-      <c r="G275" s="29"/>
+      <c r="E275" s="9"/>
+      <c r="F275" s="9"/>
+      <c r="G275" s="28"/>
     </row>
     <row r="276" spans="1:7">
-      <c r="A276" s="44">
+      <c r="A276" s="42">
         <v>44487</v>
       </c>
-      <c r="B276" s="45">
+      <c r="B276" s="43">
         <v>1.21</v>
       </c>
-      <c r="C276" s="20" t="s">
+      <c r="C276" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D276" s="46" t="s">
+      <c r="D276" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="E276" s="47"/>
-      <c r="F276" s="48"/>
-      <c r="G276" s="29"/>
+      <c r="E276" s="9"/>
+      <c r="F276" s="9"/>
+      <c r="G276" s="28"/>
     </row>
     <row r="277" spans="1:7">
-      <c r="A277" s="44">
+      <c r="A277" s="42">
         <v>44518</v>
       </c>
-      <c r="B277" s="45">
+      <c r="B277" s="43">
         <v>1.22</v>
       </c>
-      <c r="C277" s="20" t="s">
+      <c r="C277" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D277" s="46" t="s">
+      <c r="D277" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="E277" s="47"/>
-      <c r="F277" s="48"/>
-      <c r="G277" s="29"/>
+      <c r="E277" s="9"/>
+      <c r="F277" s="9"/>
+      <c r="G277" s="28"/>
     </row>
     <row r="278" spans="1:7">
-      <c r="A278" s="44">
+      <c r="A278" s="42">
         <v>44530</v>
       </c>
-      <c r="B278" s="45">
+      <c r="B278" s="43">
         <v>1.23</v>
       </c>
-      <c r="C278" s="20" t="s">
+      <c r="C278" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D278" s="46" t="s">
+      <c r="D278" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="E278" s="47"/>
-      <c r="F278" s="48"/>
-      <c r="G278" s="29"/>
+      <c r="E278" s="9"/>
+      <c r="F278" s="9"/>
+      <c r="G278" s="28"/>
     </row>
     <row r="279" spans="1:7">
-      <c r="A279" s="44">
+      <c r="A279" s="42">
         <v>44559</v>
       </c>
-      <c r="B279" s="45">
+      <c r="B279" s="43">
         <v>1.24</v>
       </c>
-      <c r="C279" s="20" t="s">
+      <c r="C279" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D279" s="46" t="s">
+      <c r="D279" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E279" s="47"/>
-      <c r="F279" s="48"/>
-      <c r="G279" s="29"/>
+      <c r="E279" s="9"/>
+      <c r="F279" s="9"/>
+      <c r="G279" s="28"/>
     </row>
     <row r="280" spans="1:7">
-      <c r="A280" s="44">
+      <c r="A280" s="42">
         <v>44755</v>
       </c>
-      <c r="B280" s="45">
+      <c r="B280" s="43">
         <v>1.25</v>
       </c>
-      <c r="C280" s="20" t="s">
+      <c r="C280" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D280" s="46" t="s">
+      <c r="D280" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="E280" s="47"/>
-      <c r="F280" s="48"/>
-      <c r="G280" s="29"/>
+      <c r="E280" s="9"/>
+      <c r="F280" s="9"/>
+      <c r="G280" s="28"/>
     </row>
     <row r="281" spans="1:7">
-      <c r="A281" s="44">
+      <c r="A281" s="42">
         <v>44881</v>
       </c>
-      <c r="B281" s="45">
+      <c r="B281" s="43">
         <v>1.26</v>
       </c>
-      <c r="C281" s="20" t="s">
+      <c r="C281" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D281" s="46" t="s">
+      <c r="D281" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="E281" s="47"/>
-      <c r="F281" s="48"/>
-      <c r="G281" s="29"/>
+      <c r="E281" s="9"/>
+      <c r="F281" s="9"/>
+      <c r="G281" s="28"/>
     </row>
     <row r="282" spans="1:7">
-      <c r="A282" s="44">
+      <c r="A282" s="42">
         <v>44955</v>
       </c>
-      <c r="B282" s="45">
+      <c r="B282" s="43">
         <v>1.27</v>
       </c>
-      <c r="C282" s="20" t="s">
+      <c r="C282" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D282" s="84" t="s">
+      <c r="D282" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="E282" s="85"/>
-      <c r="F282" s="86"/>
-      <c r="G282" s="29"/>
-    </row>
-    <row r="283" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A283" s="49">
+      <c r="E282" s="9"/>
+      <c r="F282" s="9"/>
+      <c r="G282" s="28"/>
+    </row>
+    <row r="283" spans="1:7">
+      <c r="A283" s="42">
         <v>45063</v>
       </c>
-      <c r="B283" s="50">
+      <c r="B283" s="43">
         <v>1.28</v>
       </c>
-      <c r="C283" s="24" t="s">
+      <c r="C283" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D283" s="87" t="s">
+      <c r="D283" s="57" t="s">
         <v>364</v>
       </c>
-      <c r="E283" s="88"/>
-      <c r="F283" s="89"/>
-      <c r="G283" s="30"/>
+      <c r="E283" s="9"/>
+      <c r="F283" s="9"/>
+      <c r="G283" s="28"/>
+    </row>
+    <row r="284" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A284" s="44">
+        <v>45306</v>
+      </c>
+      <c r="B284" s="45">
+        <v>1.29</v>
+      </c>
+      <c r="C284" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="D284" s="117" t="s">
+        <v>369</v>
+      </c>
+      <c r="E284" s="15"/>
+      <c r="F284" s="15"/>
+      <c r="G284" s="30"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wU2MPYQTUl5fmkHxEwxkAQgetFKupSVMNNSnprLVIZhhQGv6RD9XY6hN8ly1aOrB6DLKRMajx1q9n9FGeldF0w==" saltValue="tJLfUfosdS72lDaD9KhyrA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="yQNKhd/GHALWY3j1VdBWXAmgqOh3V2w7onCTUCjJij/FjrqwIO8vAlYRZoMBRo6i17/X7aTiP/c+3MoAtEjMWQ==" saltValue="T8uRdw4/X+G+CdjhgA1DDg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A139">
       <selection activeCell="D163" sqref="D163"/>
@@ -9609,30 +9568,16 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="50">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C229:E229"/>
-    <mergeCell ref="C230:E230"/>
-    <mergeCell ref="C231:E231"/>
-    <mergeCell ref="C232:E232"/>
-    <mergeCell ref="C233:E233"/>
-    <mergeCell ref="C234:E234"/>
-    <mergeCell ref="C235:E235"/>
-    <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C237:E237"/>
-    <mergeCell ref="C238:E238"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="C240:E240"/>
-    <mergeCell ref="C241:E241"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="B253:E253"/>
-    <mergeCell ref="B254:E254"/>
-    <mergeCell ref="D259:F259"/>
-    <mergeCell ref="D260:F260"/>
-    <mergeCell ref="C243:E243"/>
-    <mergeCell ref="C244:E244"/>
-    <mergeCell ref="C245:E245"/>
-    <mergeCell ref="B250:E250"/>
-    <mergeCell ref="B251:E251"/>
+    <mergeCell ref="B201:B203"/>
+    <mergeCell ref="B204:B212"/>
+    <mergeCell ref="B230:B231"/>
+    <mergeCell ref="B232:B233"/>
+    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="B149:B163"/>
+    <mergeCell ref="B164:B172"/>
+    <mergeCell ref="B173:B183"/>
+    <mergeCell ref="B184:B191"/>
+    <mergeCell ref="B192:B200"/>
     <mergeCell ref="D266:F266"/>
     <mergeCell ref="D267:F267"/>
     <mergeCell ref="A230:A237"/>
@@ -9649,16 +9594,30 @@
     <mergeCell ref="D264:F264"/>
     <mergeCell ref="D265:F265"/>
     <mergeCell ref="B252:E252"/>
-    <mergeCell ref="B149:B163"/>
-    <mergeCell ref="B164:B172"/>
-    <mergeCell ref="B173:B183"/>
-    <mergeCell ref="B184:B191"/>
-    <mergeCell ref="B192:B200"/>
-    <mergeCell ref="B201:B203"/>
-    <mergeCell ref="B204:B212"/>
-    <mergeCell ref="B230:B231"/>
-    <mergeCell ref="B232:B233"/>
-    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="B253:E253"/>
+    <mergeCell ref="B254:E254"/>
+    <mergeCell ref="D259:F259"/>
+    <mergeCell ref="D260:F260"/>
+    <mergeCell ref="C243:E243"/>
+    <mergeCell ref="C244:E244"/>
+    <mergeCell ref="C245:E245"/>
+    <mergeCell ref="B250:E250"/>
+    <mergeCell ref="B251:E251"/>
+    <mergeCell ref="C238:E238"/>
+    <mergeCell ref="C239:E239"/>
+    <mergeCell ref="C240:E240"/>
+    <mergeCell ref="C241:E241"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C233:E233"/>
+    <mergeCell ref="C234:E234"/>
+    <mergeCell ref="C235:E235"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="C237:E237"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="C230:E230"/>
+    <mergeCell ref="C231:E231"/>
+    <mergeCell ref="C232:E232"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -9684,16 +9643,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>